<commit_message>
Input processing completed (with timestamp format) :white_check_mark:
</commit_message>
<xml_diff>
--- a/src/InputOutput/Sample.xlsx
+++ b/src/InputOutput/Sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\github\Uni_Timetables\src\InputOutput\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\PycharmProjects\Uni_Timetables\src\InputOutput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC228BDC-F87A-4CA0-BA34-F03FC805C72F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116AD4BC-A924-421B-8026-41ACC2D224F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="118">
   <si>
     <t>Programme</t>
   </si>
@@ -65,60 +65,18 @@
     <t>BAY1</t>
   </si>
   <si>
-    <t>KEN1520</t>
-  </si>
-  <si>
-    <t>SE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Software Engineering </t>
-  </si>
-  <si>
-    <t>T.Pepels; C.Seiler</t>
-  </si>
-  <si>
     <t>BAY2</t>
   </si>
   <si>
-    <t>KEN1530</t>
-  </si>
-  <si>
-    <t>LO</t>
-  </si>
-  <si>
-    <t>Logic</t>
-  </si>
-  <si>
-    <t>J. Uiterwijk; N. Roos</t>
-  </si>
-  <si>
     <t>BAY3</t>
   </si>
   <si>
-    <t>KEN1540</t>
-  </si>
-  <si>
-    <t>NUM</t>
-  </si>
-  <si>
-    <t>Numerical Mathematics</t>
-  </si>
-  <si>
-    <t>K. Schüller; S.Maryam; C.Sironi</t>
-  </si>
-  <si>
     <t>MAAIY1</t>
   </si>
   <si>
-    <t>MAAIY2</t>
-  </si>
-  <si>
     <t>MADSDMY1</t>
   </si>
   <si>
-    <t>MADSDMY2</t>
-  </si>
-  <si>
     <t>Lecturer</t>
   </si>
   <si>
@@ -140,37 +98,295 @@
     <t>RoomID</t>
   </si>
   <si>
-    <t>KEN1550</t>
-  </si>
-  <si>
-    <t>KEN1551</t>
-  </si>
-  <si>
-    <t>KEN1552</t>
-  </si>
-  <si>
-    <t>KEN1553</t>
-  </si>
-  <si>
     <t>Paul</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Is </t>
-  </si>
-  <si>
-    <t>Dannnniel</t>
-  </si>
-  <si>
-    <t>Blub</t>
+    <t>KEN1110</t>
+  </si>
+  <si>
+    <t>KEN1120</t>
+  </si>
+  <si>
+    <t>KEN1130</t>
+  </si>
+  <si>
+    <t>KEN1300</t>
+  </si>
+  <si>
+    <t>Introduction to Data Science and Knowledge Engineering</t>
+  </si>
+  <si>
+    <t>IKE</t>
+  </si>
+  <si>
+    <t>CSI</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>Introduction to Computer Science</t>
+  </si>
+  <si>
+    <t>Discrete Mathematics</t>
+  </si>
+  <si>
+    <t>Project Meeting</t>
+  </si>
+  <si>
+    <t>KEN2110</t>
+  </si>
+  <si>
+    <t>KEN2120</t>
+  </si>
+  <si>
+    <t>KEN2130</t>
+  </si>
+  <si>
+    <t>P&amp;AI</t>
+  </si>
+  <si>
+    <t>P&amp;S</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Databases</t>
+  </si>
+  <si>
+    <t>Philosophy &amp; Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>Probability &amp; Statistics</t>
+  </si>
+  <si>
+    <t>P. Bonizzi; R. Cavill</t>
+  </si>
+  <si>
+    <t>E. Hortal Quesada; J. Spanakis</t>
+  </si>
+  <si>
+    <t>S. Kelk; M. Mihalak</t>
+  </si>
+  <si>
+    <t>K. Schüller; M. Popa</t>
+  </si>
+  <si>
+    <t>D. Rafailidis</t>
+  </si>
+  <si>
+    <t>D. Cressman; K. Gabriels</t>
+  </si>
+  <si>
+    <t>C. Seiler</t>
+  </si>
+  <si>
+    <t>KEN2300</t>
+  </si>
+  <si>
+    <t>K. Schüller; J. Uiterwijk; M. Mihalak</t>
+  </si>
+  <si>
+    <t>KEN3140</t>
+  </si>
+  <si>
+    <t>KEN2560</t>
+  </si>
+  <si>
+    <t>Elective</t>
+  </si>
+  <si>
+    <t>KEN3234</t>
+  </si>
+  <si>
+    <t>KEN3130</t>
+  </si>
+  <si>
+    <t>KEN3236</t>
+  </si>
+  <si>
+    <t>KEN3300</t>
+  </si>
+  <si>
+    <t>PROLOG</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>GT</t>
+  </si>
+  <si>
+    <t>RES</t>
+  </si>
+  <si>
+    <t>Prolog</t>
+  </si>
+  <si>
+    <t>Computer Security</t>
+  </si>
+  <si>
+    <t>Semantic Web</t>
+  </si>
+  <si>
+    <t>Game Theory</t>
+  </si>
+  <si>
+    <t>Robotics and Embedded Systems</t>
+  </si>
+  <si>
+    <t>J. Uiterwijk</t>
+  </si>
+  <si>
+    <t>A. Zarras</t>
+  </si>
+  <si>
+    <t>N. Roos; M. Dumontier</t>
+  </si>
+  <si>
+    <t>F. Thuijsman</t>
+  </si>
+  <si>
+    <t>R. Möckel</t>
+  </si>
+  <si>
+    <t>KEN4115</t>
+  </si>
+  <si>
+    <t>KEN4123</t>
+  </si>
+  <si>
+    <t>KEN4113</t>
+  </si>
+  <si>
+    <t>KEN2111</t>
+  </si>
+  <si>
+    <t>KEN4221</t>
+  </si>
+  <si>
+    <t>KEN4222</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>ISG</t>
+  </si>
+  <si>
+    <t>OPT</t>
+  </si>
+  <si>
+    <t>SIP</t>
+  </si>
+  <si>
+    <t>SDM</t>
+  </si>
+  <si>
+    <t>KEN4130</t>
+  </si>
+  <si>
+    <t>Foundations of Agents</t>
+  </si>
+  <si>
+    <t>Intelligent Search &amp; Games</t>
+  </si>
+  <si>
+    <t>Data Mining</t>
+  </si>
+  <si>
+    <t>Mathematical Optimization</t>
+  </si>
+  <si>
+    <t>Signal and Image Processing</t>
+  </si>
+  <si>
+    <t>Stochastic Decision Making</t>
+  </si>
+  <si>
+    <t>N. Roos</t>
+  </si>
+  <si>
+    <t>M. Winands; C. Browne</t>
+  </si>
+  <si>
+    <t>E. Smirnov</t>
+  </si>
+  <si>
+    <t>P. Collins</t>
+  </si>
+  <si>
+    <t>J. Karel; P. Bonizzi</t>
+  </si>
+  <si>
+    <t>G. Schoenmakers</t>
+  </si>
+  <si>
+    <t>K. Driessens</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>Deep Space</t>
+  </si>
+  <si>
+    <t>Cyberspace</t>
+  </si>
+  <si>
+    <t>Search Space</t>
+  </si>
+  <si>
+    <t>Eigenspace</t>
+  </si>
+  <si>
+    <t>Vector Space</t>
+  </si>
+  <si>
+    <t>Memory Space</t>
+  </si>
+  <si>
+    <t>Black Box</t>
+  </si>
+  <si>
+    <t>Glass Box</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -211,15 +427,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -438,9 +655,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -450,6 +669,14 @@
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>43710</v>
+      </c>
+      <c r="B2" s="5">
+        <v>43764</v>
       </c>
     </row>
   </sheetData>
@@ -462,15 +689,27 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>43723</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>43728</v>
       </c>
     </row>
   </sheetData>
@@ -483,19 +722,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,112 +756,560 @@
       <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="2">
+        <v>36</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="2">
+        <v>125</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="2">
+        <v>36</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="2">
+        <v>125</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="2">
+        <v>36</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="2">
+        <v>125</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="2">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="2">
+        <v>125</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="2">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="2">
+        <v>100</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="2">
+        <v>36</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="2">
+        <v>100</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="2">
+        <v>36</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="2">
+        <v>100</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="2">
+        <v>22</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="2">
+        <v>100</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="2">
+        <v>36</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="2">
+        <v>75</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="2">
+        <v>36</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="2">
+        <v>75</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="2">
+        <v>36</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="2">
+        <v>75</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="2">
+        <v>36</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="2">
+        <v>75</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="2">
+        <v>36</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" s="2">
+        <v>75</v>
+      </c>
+      <c r="H14" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="2">
+        <v>20</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="2">
+        <v>75</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="2">
-        <v>35</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="B16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="2">
+        <v>34</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" s="2">
+        <v>50</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="2">
+        <v>34</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" s="2">
+        <v>50</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="2">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B18" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="2">
+        <v>34</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="2">
+        <v>50</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="2">
+        <v>34</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="2">
+        <v>50</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" s="2">
+        <v>34</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" s="2">
+        <v>50</v>
+      </c>
+      <c r="H20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="2">
+        <v>34</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G21" s="2">
+        <v>50</v>
+      </c>
+      <c r="H21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="2">
         <v>20</v>
       </c>
-      <c r="E3" s="2">
-        <v>34</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="2">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="2">
-        <v>35</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="2">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>41</v>
+      <c r="F22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" s="2">
+        <v>50</v>
+      </c>
+      <c r="H22" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -636,21 +1323,111 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>33</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -666,124 +1443,125 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:D8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="7">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3">
         <v>43941</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="6">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="7">
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="7">
-        <v>43941</v>
-      </c>
-      <c r="C3" s="4">
+        <v>22</v>
+      </c>
+      <c r="B3" s="3">
+        <v>43942</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.64583333333333337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3">
+        <v>43943</v>
+      </c>
+      <c r="C4" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D3" s="4">
-        <v>0.64583333333333337</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="D4" s="7">
         <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="4">
+        <v>22</v>
+      </c>
+      <c r="B5" s="3">
+        <v>43944</v>
+      </c>
+      <c r="C5" s="7">
         <v>0.625</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="7">
         <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="5">
+        <v>22</v>
+      </c>
+      <c r="B6" s="3">
+        <v>43945</v>
+      </c>
+      <c r="C6" s="8">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="8">
         <v>0.65277777777777779</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="5">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3">
+        <v>43946</v>
+      </c>
+      <c r="C7" s="8">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="8">
         <v>0.65277777777777779</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="5">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3">
+        <v>43947</v>
+      </c>
+      <c r="C8" s="8">
         <v>0.54166666666666663</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="8">
         <v>0.65277777777777779</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Very simple greedy algorithm done :rocket:
</commit_message>
<xml_diff>
--- a/src/InputOutput/Sample.xlsx
+++ b/src/InputOutput/Sample.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\PycharmProjects\Uni_Timetables\src\InputOutput\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\github\Uni_Timetables\src\InputOutput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116AD4BC-A924-421B-8026-41ACC2D224F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47713B1B-B419-4098-86AE-B71872241437}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PeriodInfo" sheetId="1" r:id="rId1"/>
@@ -385,7 +385,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -434,9 +434,9 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -663,7 +663,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -697,7 +697,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -724,8 +724,8 @@
   </sheetPr>
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -734,7 +734,7 @@
     <col min="10" max="10" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -766,7 +766,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -792,7 +792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -818,7 +818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -844,7 +844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -870,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -896,7 +896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -922,7 +922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -948,7 +948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -974,7 +974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1326,12 +1326,12 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
@@ -1442,7 +1442,7 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
1st ILP producing schedules :poop::ok_hand:
Basic ILP producing a schedule (with given contact hours as the onlzyconstraint)

Co-Authored-By: dexter192 <dexter192@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/InputOutput/Sample.xlsx
+++ b/src/InputOutput/Sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\github\Uni_Timetables\src\InputOutput\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul Disbeschl\Documents\GitHub\Uni_Timetables\src\InputOutput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47713B1B-B419-4098-86AE-B71872241437}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D73E56-9A39-4838-9B12-76C38EFE4E97}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PeriodInfo" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,15 @@
     <sheet name="Rooms" sheetId="4" r:id="rId4"/>
     <sheet name="Lecturers" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -439,7 +447,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -661,7 +669,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -691,11 +699,11 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -704,7 +712,7 @@
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
-        <v>43723</v>
+        <v>43721</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -724,11 +732,11 @@
   </sheetPr>
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="15.140625" customWidth="1"/>
@@ -1329,7 +1337,7 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1446,7 +1454,7 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
More ILP hard-constraints :boom: :alembic:
ILP considers lecture lap of years, overlap of teachers and unavailability of teachers
</commit_message>
<xml_diff>
--- a/src/InputOutput/Sample.xlsx
+++ b/src/InputOutput/Sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul Disbeschl\Documents\GitHub\Uni_Timetables\src\InputOutput\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\PycharmProjects\Uni_Timetables\src\InputOutput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D73E56-9A39-4838-9B12-76C38EFE4E97}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E925218-0A6A-44DF-9B26-E693AFE801DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PeriodInfo" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="120">
   <si>
     <t>Programme</t>
   </si>
@@ -386,6 +386,12 @@
   </si>
   <si>
     <t>Glass Box</t>
+  </si>
+  <si>
+    <t>P. Bonizzi</t>
+  </si>
+  <si>
+    <t>R.Möckel</t>
   </si>
 </sst>
 </file>
@@ -395,7 +401,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -414,6 +420,12 @@
       <sz val="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -423,7 +435,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -431,11 +443,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -445,9 +472,12 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -669,7 +699,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -699,11 +729,11 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -733,10 +763,10 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="15.140625" customWidth="1"/>
@@ -1337,7 +1367,7 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1448,13 +1478,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1471,11 +1501,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>22</v>
+      <c r="A2" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="B2" s="3">
-        <v>43941</v>
+        <v>43713</v>
       </c>
       <c r="C2" s="6">
         <v>0.33333333333333331</v>
@@ -1485,11 +1515,11 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
+      <c r="A3" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="B3" s="3">
-        <v>43942</v>
+        <v>43713</v>
       </c>
       <c r="C3" s="7">
         <v>0.35416666666666669</v>
@@ -1499,17 +1529,17 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
+      <c r="A4" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="B4" s="3">
-        <v>43943</v>
+        <v>43710</v>
       </c>
       <c r="C4" s="7">
         <v>0.33333333333333331</v>
       </c>
       <c r="D4" s="7">
-        <v>0.54166666666666663</v>
+        <v>0.5625</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1517,7 +1547,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="3">
-        <v>43944</v>
+        <v>43716</v>
       </c>
       <c r="C5" s="7">
         <v>0.625</v>
@@ -1531,7 +1561,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="3">
-        <v>43945</v>
+        <v>43717</v>
       </c>
       <c r="C6" s="8">
         <v>0.54166666666666663</v>
@@ -1545,7 +1575,7 @@
         <v>24</v>
       </c>
       <c r="B7" s="3">
-        <v>43946</v>
+        <v>43718</v>
       </c>
       <c r="C7" s="8">
         <v>0.54166666666666663</v>
@@ -1559,17 +1589,32 @@
         <v>24</v>
       </c>
       <c r="B8" s="3">
-        <v>43947</v>
+        <v>43719</v>
       </c>
       <c r="C8" s="8">
         <v>0.54166666666666663</v>
       </c>
       <c r="D8" s="8">
         <v>0.65277777777777779</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="3">
+        <v>43712</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.35486111111111113</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/pdisbeschl/Uni_Timetables"
This reverts commit 68d1401bab4bada728d9c89b6586b0391556ed6a, reversing
changes made to 2b7c990b1ccf6950327600331acd72cfc81c8664.
</commit_message>
<xml_diff>
--- a/src/InputOutput/Sample.xlsx
+++ b/src/InputOutput/Sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\PycharmProjects\Uni_Timetables\src\InputOutput\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul Disbeschl\Documents\GitHub\Uni_Timetables\src\InputOutput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E925218-0A6A-44DF-9B26-E693AFE801DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D73E56-9A39-4838-9B12-76C38EFE4E97}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PeriodInfo" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="118">
   <si>
     <t>Programme</t>
   </si>
@@ -386,12 +386,6 @@
   </si>
   <si>
     <t>Glass Box</t>
-  </si>
-  <si>
-    <t>P. Bonizzi</t>
-  </si>
-  <si>
-    <t>R.Möckel</t>
   </si>
 </sst>
 </file>
@@ -401,7 +395,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -420,12 +414,6 @@
       <sz val="8"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -435,7 +423,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -443,26 +431,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -472,12 +445,9 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -699,7 +669,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -729,11 +699,11 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -763,10 +733,10 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="15.140625" customWidth="1"/>
@@ -1367,7 +1337,7 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1478,13 +1448,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1501,11 +1471,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>118</v>
+      <c r="A2" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B2" s="3">
-        <v>43713</v>
+        <v>43941</v>
       </c>
       <c r="C2" s="6">
         <v>0.33333333333333331</v>
@@ -1515,11 +1485,11 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>118</v>
+      <c r="A3" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B3" s="3">
-        <v>43713</v>
+        <v>43942</v>
       </c>
       <c r="C3" s="7">
         <v>0.35416666666666669</v>
@@ -1529,17 +1499,17 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>118</v>
+      <c r="A4" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B4" s="3">
-        <v>43710</v>
+        <v>43943</v>
       </c>
       <c r="C4" s="7">
         <v>0.33333333333333331</v>
       </c>
       <c r="D4" s="7">
-        <v>0.5625</v>
+        <v>0.54166666666666663</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1547,7 +1517,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="3">
-        <v>43716</v>
+        <v>43944</v>
       </c>
       <c r="C5" s="7">
         <v>0.625</v>
@@ -1561,7 +1531,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="3">
-        <v>43717</v>
+        <v>43945</v>
       </c>
       <c r="C6" s="8">
         <v>0.54166666666666663</v>
@@ -1575,7 +1545,7 @@
         <v>24</v>
       </c>
       <c r="B7" s="3">
-        <v>43718</v>
+        <v>43946</v>
       </c>
       <c r="C7" s="8">
         <v>0.54166666666666663</v>
@@ -1589,32 +1559,17 @@
         <v>24</v>
       </c>
       <c r="B8" s="3">
-        <v>43719</v>
+        <v>43947</v>
       </c>
       <c r="C8" s="8">
         <v>0.54166666666666663</v>
       </c>
       <c r="D8" s="8">
         <v>0.65277777777777779</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" s="3">
-        <v>43712</v>
-      </c>
-      <c r="C9" s="8">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="D9" s="8">
-        <v>0.35486111111111113</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing the mess I made
</commit_message>
<xml_diff>
--- a/src/InputOutput/Sample.xlsx
+++ b/src/InputOutput/Sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul Disbeschl\Documents\GitHub\Uni_Timetables\src\InputOutput\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\PycharmProjects\Uni_Timetables\src\InputOutput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D73E56-9A39-4838-9B12-76C38EFE4E97}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E925218-0A6A-44DF-9B26-E693AFE801DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PeriodInfo" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="120">
   <si>
     <t>Programme</t>
   </si>
@@ -386,6 +386,12 @@
   </si>
   <si>
     <t>Glass Box</t>
+  </si>
+  <si>
+    <t>P. Bonizzi</t>
+  </si>
+  <si>
+    <t>R.Möckel</t>
   </si>
 </sst>
 </file>
@@ -395,7 +401,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -414,6 +420,12 @@
       <sz val="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -423,7 +435,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -431,11 +443,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -445,9 +472,12 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -669,7 +699,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -699,11 +729,11 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
@@ -733,10 +763,10 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="15.140625" customWidth="1"/>
@@ -1337,7 +1367,7 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1448,13 +1478,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1471,11 +1501,11 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>22</v>
+      <c r="A2" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="B2" s="3">
-        <v>43941</v>
+        <v>43713</v>
       </c>
       <c r="C2" s="6">
         <v>0.33333333333333331</v>
@@ -1485,11 +1515,11 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>22</v>
+      <c r="A3" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="B3" s="3">
-        <v>43942</v>
+        <v>43713</v>
       </c>
       <c r="C3" s="7">
         <v>0.35416666666666669</v>
@@ -1499,17 +1529,17 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>22</v>
+      <c r="A4" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="B4" s="3">
-        <v>43943</v>
+        <v>43710</v>
       </c>
       <c r="C4" s="7">
         <v>0.33333333333333331</v>
       </c>
       <c r="D4" s="7">
-        <v>0.54166666666666663</v>
+        <v>0.5625</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1517,7 +1547,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="3">
-        <v>43944</v>
+        <v>43716</v>
       </c>
       <c r="C5" s="7">
         <v>0.625</v>
@@ -1531,7 +1561,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="3">
-        <v>43945</v>
+        <v>43717</v>
       </c>
       <c r="C6" s="8">
         <v>0.54166666666666663</v>
@@ -1545,7 +1575,7 @@
         <v>24</v>
       </c>
       <c r="B7" s="3">
-        <v>43946</v>
+        <v>43718</v>
       </c>
       <c r="C7" s="8">
         <v>0.54166666666666663</v>
@@ -1559,17 +1589,32 @@
         <v>24</v>
       </c>
       <c r="B8" s="3">
-        <v>43947</v>
+        <v>43719</v>
       </c>
       <c r="C8" s="8">
         <v>0.54166666666666663</v>
       </c>
       <c r="D8" s="8">
         <v>0.65277777777777779</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="3">
+        <v>43712</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.35486111111111113</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
:sparkles: Entries in a schedule are now clickable and course info is schown and the schedule is downloadable in json format
</commit_message>
<xml_diff>
--- a/src/InputOutput/Sample.xlsx
+++ b/src/InputOutput/Sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\PycharmProjects\Uni_Timetables\src\InputOutput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E925218-0A6A-44DF-9B26-E693AFE801DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E33572B-38CA-4A45-9D98-3F9290E6D0BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PeriodInfo" sheetId="1" r:id="rId1"/>
@@ -1363,8 +1363,8 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1480,7 +1480,7 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
:sparkles: Timeslots are now highlighted based on availability when swapping
</commit_message>
<xml_diff>
--- a/src/InputOutput/Sample.xlsx
+++ b/src/InputOutput/Sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\PycharmProjects\Uni_Timetables\src\InputOutput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E33572B-38CA-4A45-9D98-3F9290E6D0BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADF327C-2A25-4C40-997C-1A0A90686058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4335" yWindow="690" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PeriodInfo" sheetId="1" r:id="rId1"/>
@@ -184,9 +184,6 @@
     <t>K. Schüller; M. Popa</t>
   </si>
   <si>
-    <t>D. Rafailidis</t>
-  </si>
-  <si>
     <t>D. Cressman; K. Gabriels</t>
   </si>
   <si>
@@ -392,6 +389,9 @@
   </si>
   <si>
     <t>R.Möckel</t>
+  </si>
+  <si>
+    <t>R. Cavill</t>
   </si>
 </sst>
 </file>
@@ -762,8 +762,8 @@
   </sheetPr>
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -795,7 +795,7 @@
         <v>9</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>10</v>
@@ -925,7 +925,7 @@
         <v>36</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="G6" s="2">
         <v>100</v>
@@ -951,7 +951,7 @@
         <v>36</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G7" s="2">
         <v>100</v>
@@ -977,7 +977,7 @@
         <v>36</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G8" s="2">
         <v>100</v>
@@ -991,7 +991,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>33</v>
@@ -1003,7 +1003,7 @@
         <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G9" s="2">
         <v>100</v>
@@ -1017,19 +1017,19 @@
         <v>14</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="2">
         <v>36</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G10" s="2">
         <v>75</v>
@@ -1043,19 +1043,19 @@
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11" s="2">
         <v>36</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G11" s="2">
         <v>75</v>
@@ -1069,19 +1069,19 @@
         <v>14</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" s="2">
         <v>36</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G12" s="2">
         <v>75</v>
@@ -1095,19 +1095,19 @@
         <v>14</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E13" s="2">
         <v>36</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G13" s="2">
         <v>75</v>
@@ -1121,19 +1121,19 @@
         <v>14</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E14" s="2">
         <v>36</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G14" s="2">
         <v>75</v>
@@ -1147,7 +1147,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>33</v>
@@ -1159,7 +1159,7 @@
         <v>20</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G15" s="2">
         <v>75</v>
@@ -1173,19 +1173,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E16" s="2">
         <v>34</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G16" s="2">
         <v>50</v>
@@ -1199,19 +1199,19 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E17" s="2">
         <v>34</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G17" s="2">
         <v>50</v>
@@ -1225,19 +1225,19 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E18" s="2">
         <v>34</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G18" s="2">
         <v>50</v>
@@ -1251,19 +1251,19 @@
         <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E19" s="2">
         <v>34</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G19" s="2">
         <v>50</v>
@@ -1277,19 +1277,19 @@
         <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E20" s="2">
         <v>34</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G20" s="2">
         <v>50</v>
@@ -1303,19 +1303,19 @@
         <v>16</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E21" s="2">
         <v>34</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G21" s="2">
         <v>50</v>
@@ -1329,7 +1329,7 @@
         <v>16</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>33</v>
@@ -1341,7 +1341,7 @@
         <v>20</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G22" s="2">
         <v>50</v>
@@ -1363,7 +1363,7 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -1382,10 +1382,10 @@
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C2">
         <v>150</v>
@@ -1393,10 +1393,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C3">
         <v>150</v>
@@ -1404,10 +1404,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C4">
         <v>150</v>
@@ -1415,10 +1415,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C5">
         <v>150</v>
@@ -1426,10 +1426,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6">
         <v>150</v>
@@ -1437,10 +1437,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7">
         <v>150</v>
@@ -1448,10 +1448,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C8">
         <v>100</v>
@@ -1459,10 +1459,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9">
         <v>100</v>
@@ -1502,7 +1502,7 @@
     </row>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" s="3">
         <v>43713</v>
@@ -1516,7 +1516,7 @@
     </row>
     <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="3">
         <v>43713</v>
@@ -1530,7 +1530,7 @@
     </row>
     <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="3">
         <v>43710</v>
@@ -1600,7 +1600,7 @@
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B9" s="3">
         <v>43712</v>

</xml_diff>

<commit_message>
:sparkles: Courses can now be edited
</commit_message>
<xml_diff>
--- a/src/InputOutput/Sample.xlsx
+++ b/src/InputOutput/Sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\PycharmProjects\Uni_Timetables\src\InputOutput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FADF327C-2A25-4C40-997C-1A0A90686058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E9CE7D-7CAF-4FEF-AA39-C20DED196D97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4335" yWindow="690" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PeriodInfo" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="118">
   <si>
     <t>Programme</t>
   </si>
@@ -62,12 +62,6 @@
   </si>
   <si>
     <t>Number of students</t>
-  </si>
-  <si>
-    <t>SpecialDuration*</t>
-  </si>
-  <si>
-    <t>SpecialFacilities*</t>
   </si>
   <si>
     <t>BAY1</t>
@@ -762,8 +756,8 @@
   </sheetPr>
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -795,33 +789,29 @@
         <v>9</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E2" s="2">
         <v>36</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G2" s="2">
         <v>125</v>
@@ -832,22 +822,22 @@
     </row>
     <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E3" s="2">
         <v>36</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G3" s="2">
         <v>125</v>
@@ -858,22 +848,22 @@
     </row>
     <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E4" s="2">
         <v>36</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G4" s="2">
         <v>125</v>
@@ -884,22 +874,22 @@
     </row>
     <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E5" s="2">
         <v>12</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G5" s="2">
         <v>125</v>
@@ -910,22 +900,22 @@
     </row>
     <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E6" s="2">
         <v>36</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G6" s="2">
         <v>100</v>
@@ -936,22 +926,22 @@
     </row>
     <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E7" s="2">
         <v>36</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G7" s="2">
         <v>100</v>
@@ -962,22 +952,22 @@
     </row>
     <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E8" s="2">
         <v>36</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G8" s="2">
         <v>100</v>
@@ -988,22 +978,22 @@
     </row>
     <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2">
         <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G9" s="2">
         <v>100</v>
@@ -1014,22 +1004,22 @@
     </row>
     <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E10" s="2">
         <v>36</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G10" s="2">
         <v>75</v>
@@ -1040,22 +1030,22 @@
     </row>
     <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E11" s="2">
         <v>36</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G11" s="2">
         <v>75</v>
@@ -1066,22 +1056,22 @@
     </row>
     <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E12" s="2">
         <v>36</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G12" s="2">
         <v>75</v>
@@ -1092,22 +1082,22 @@
     </row>
     <row r="13" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E13" s="2">
         <v>36</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G13" s="2">
         <v>75</v>
@@ -1118,22 +1108,22 @@
     </row>
     <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E14" s="2">
         <v>36</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G14" s="2">
         <v>75</v>
@@ -1144,22 +1134,22 @@
     </row>
     <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E15" s="2">
         <v>20</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G15" s="2">
         <v>75</v>
@@ -1170,22 +1160,22 @@
     </row>
     <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E16" s="2">
         <v>34</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G16" s="2">
         <v>50</v>
@@ -1196,22 +1186,22 @@
     </row>
     <row r="17" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E17" s="2">
         <v>34</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G17" s="2">
         <v>50</v>
@@ -1222,22 +1212,22 @@
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E18" s="2">
         <v>34</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G18" s="2">
         <v>50</v>
@@ -1248,22 +1238,22 @@
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E19" s="2">
         <v>34</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G19" s="2">
         <v>50</v>
@@ -1274,22 +1264,22 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E20" s="2">
         <v>34</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G20" s="2">
         <v>50</v>
@@ -1300,22 +1290,22 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E21" s="2">
         <v>34</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G21" s="2">
         <v>50</v>
@@ -1326,22 +1316,22 @@
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E22" s="2">
         <v>20</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G22" s="2">
         <v>50</v>
@@ -1371,21 +1361,21 @@
   <sheetData>
     <row r="1" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C2">
         <v>150</v>
@@ -1393,10 +1383,10 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C3">
         <v>150</v>
@@ -1404,10 +1394,10 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C4">
         <v>150</v>
@@ -1415,10 +1405,10 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C5">
         <v>150</v>
@@ -1426,10 +1416,10 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C6">
         <v>150</v>
@@ -1437,10 +1427,10 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C7">
         <v>150</v>
@@ -1448,10 +1438,10 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C8">
         <v>100</v>
@@ -1459,10 +1449,10 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C9">
         <v>100</v>
@@ -1488,21 +1478,21 @@
   <sheetData>
     <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" s="3">
         <v>43713</v>
@@ -1516,7 +1506,7 @@
     </row>
     <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B3" s="3">
         <v>43713</v>
@@ -1530,7 +1520,7 @@
     </row>
     <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B4" s="3">
         <v>43710</v>
@@ -1544,7 +1534,7 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3">
         <v>43716</v>
@@ -1558,7 +1548,7 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3">
         <v>43717</v>
@@ -1572,7 +1562,7 @@
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="3">
         <v>43718</v>
@@ -1586,7 +1576,7 @@
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3">
         <v>43719</v>
@@ -1600,7 +1590,7 @@
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B9" s="3">
         <v>43712</v>

</xml_diff>